<commit_message>
changed some times added additional info to activities
</commit_message>
<xml_diff>
--- a/course_schedule.xlsx
+++ b/course_schedule.xlsx
@@ -56,18 +56,12 @@
     <t>Introduction to GitHub: Best practices in workflow management</t>
   </si>
   <si>
-    <t>Logic and data queries</t>
-  </si>
-  <si>
     <t>Course introduction</t>
   </si>
   <si>
     <t>Generating reports with rMarkdown and Notebooks</t>
   </si>
   <si>
-    <t>Avoiding repetition and for loops with purrr</t>
-  </si>
-  <si>
     <t>Strings and things: Common problem values and how to handle them</t>
   </si>
   <si>
@@ -86,12 +80,6 @@
     <t>Advanced ggPlot and an introduction to ggVis</t>
   </si>
   <si>
-    <t>Best practices in writing and managing code</t>
-  </si>
-  <si>
-    <t>Rethinking our reporting habits: New tools for managing reports</t>
-  </si>
-  <si>
     <t>Course survey</t>
   </si>
   <si>
@@ -117,13 +105,25 @@
   </si>
   <si>
     <t>Putting it all together: A cradle-to-grave data science workflow in R</t>
+  </si>
+  <si>
+    <t>Query data with indexing and logic</t>
+  </si>
+  <si>
+    <t>Rethinking our reporting habits: New tools for reporting data</t>
+  </si>
+  <si>
+    <t>Avoiding repetition and for loops with dpylr and purrr</t>
+  </si>
+  <si>
+    <t>Don't store that value! Best practices in writing &amp; managing code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,19 +140,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -189,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,22 +190,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,7 +488,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,253 +506,253 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.59375</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0.59375</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="F13" s="8"/>
+      <c r="F13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>